<commit_message>
updated stock list and processing code
updated stock list and processing code
</commit_message>
<xml_diff>
--- a/src/data/stocks.xlsx
+++ b/src/data/stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Stocks\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35D89BF-D303-4559-9B52-D51E3EE981FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ED729F-1C26-4442-9F83-E392878508A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$152</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="432">
   <si>
     <t>STOCK_NAME</t>
   </si>
@@ -699,9 +699,6 @@
     <t>SANDHAR</t>
   </si>
   <si>
-    <t>MODINATUR</t>
-  </si>
-  <si>
     <t>BIKAJI</t>
   </si>
   <si>
@@ -816,9 +813,6 @@
     <t>EXIDEIND</t>
   </si>
   <si>
-    <t>DEEPAKSP</t>
-  </si>
-  <si>
     <t>COSMOFIRST</t>
   </si>
   <si>
@@ -1041,10 +1035,295 @@
     <t>PGEL</t>
   </si>
   <si>
-    <t>TINNARUBR</t>
-  </si>
-  <si>
-    <t>VIPULORG</t>
+    <t>COLPAL</t>
+  </si>
+  <si>
+    <t>MAXHEALTH</t>
+  </si>
+  <si>
+    <t>BERGEPAINT</t>
+  </si>
+  <si>
+    <t>BAYERCROP</t>
+  </si>
+  <si>
+    <t>BASF</t>
+  </si>
+  <si>
+    <t>JCHAC</t>
+  </si>
+  <si>
+    <t>POWERINDIA</t>
+  </si>
+  <si>
+    <t>JASH</t>
+  </si>
+  <si>
+    <t>CENTURYPLY</t>
+  </si>
+  <si>
+    <t>CERA</t>
+  </si>
+  <si>
+    <t>KAJARIACER</t>
+  </si>
+  <si>
+    <t>REDINGTON</t>
+  </si>
+  <si>
+    <t>CEATLTD</t>
+  </si>
+  <si>
+    <t>MRF</t>
+  </si>
+  <si>
+    <t>TIMEX</t>
+  </si>
+  <si>
+    <t>KDDL</t>
+  </si>
+  <si>
+    <t>RAILTEL</t>
+  </si>
+  <si>
+    <t>MANKIND</t>
+  </si>
+  <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>DIVISLAB</t>
+  </si>
+  <si>
+    <t>JAICORPLTD</t>
+  </si>
+  <si>
+    <t>EPL</t>
+  </si>
+  <si>
+    <t>GRWRHITECH</t>
+  </si>
+  <si>
+    <t>TIMETECHNO</t>
+  </si>
+  <si>
+    <t>FINCABLES</t>
+  </si>
+  <si>
+    <t>SUPREMEIND</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>GMRP&amp;UI</t>
+  </si>
+  <si>
+    <t>IWEL</t>
+  </si>
+  <si>
+    <t>INOXGREEN</t>
+  </si>
+  <si>
+    <t>NAVA</t>
+  </si>
+  <si>
+    <t>WAAREERTL</t>
+  </si>
+  <si>
+    <t>CESC</t>
+  </si>
+  <si>
+    <t>HONAUT</t>
+  </si>
+  <si>
+    <t>SJVN</t>
+  </si>
+  <si>
+    <t>TORNTPOWER</t>
+  </si>
+  <si>
+    <t>NHPC</t>
+  </si>
+  <si>
+    <t>MPSLTD</t>
+  </si>
+  <si>
+    <t>RTNINDIA</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>JWL</t>
+  </si>
+  <si>
+    <t>TEXINFRA</t>
+  </si>
+  <si>
+    <t>TEXRAIL</t>
+  </si>
+  <si>
+    <t>ICRA</t>
+  </si>
+  <si>
+    <t>CRISIL</t>
+  </si>
+  <si>
+    <t>CHENNPETRO</t>
+  </si>
+  <si>
+    <t>MRPL</t>
+  </si>
+  <si>
+    <t>BPCL</t>
+  </si>
+  <si>
+    <t>IFGLEXPOR</t>
+  </si>
+  <si>
+    <t>VESUVIUS</t>
+  </si>
+  <si>
+    <t>RHIM</t>
+  </si>
+  <si>
+    <t>ETHOSLTD</t>
+  </si>
+  <si>
+    <t>ARVSMART</t>
+  </si>
+  <si>
+    <t>SHOPERSTOP</t>
+  </si>
+  <si>
+    <t>VMART</t>
+  </si>
+  <si>
+    <t>METROBRAND</t>
+  </si>
+  <si>
+    <t>APCOTEXIND</t>
+  </si>
+  <si>
+    <t>GRSE</t>
+  </si>
+  <si>
+    <t>COCHINSHIP</t>
+  </si>
+  <si>
+    <t>SEAMECLTD</t>
+  </si>
+  <si>
+    <t>SCI</t>
+  </si>
+  <si>
+    <t>GESHIP</t>
+  </si>
+  <si>
+    <t>GAEL</t>
+  </si>
+  <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>KIRLPNU</t>
+  </si>
+  <si>
+    <t>KIRLFER</t>
+  </si>
+  <si>
+    <t>KIRLOSENG</t>
+  </si>
+  <si>
+    <t>KIRLOSIND</t>
+  </si>
+  <si>
+    <t>KIRLOSBROS</t>
+  </si>
+  <si>
+    <t>MSUMI</t>
+  </si>
+  <si>
+    <t>TATASTEEL</t>
+  </si>
+  <si>
+    <t>JSWSTEEL</t>
+  </si>
+  <si>
+    <t>BANARISUG</t>
+  </si>
+  <si>
+    <t>TRIVENI</t>
+  </si>
+  <si>
+    <t>EIDPARRY</t>
+  </si>
+  <si>
+    <t>CCL</t>
+  </si>
+  <si>
+    <t>BBOX</t>
+  </si>
+  <si>
+    <t>TEJASNET</t>
+  </si>
+  <si>
+    <t>ITI</t>
+  </si>
+  <si>
+    <t>PDSL</t>
+  </si>
+  <si>
+    <t>GARFIBRES</t>
+  </si>
+  <si>
+    <t>PAGEIND</t>
+  </si>
+  <si>
+    <t>LMW</t>
+  </si>
+  <si>
+    <t>GANECOS</t>
+  </si>
+  <si>
+    <t>TRIDENT</t>
+  </si>
+  <si>
+    <t>SANOFI</t>
+  </si>
+  <si>
+    <t>NEULANDLAB</t>
+  </si>
+  <si>
+    <t>ASTRAZEN</t>
+  </si>
+  <si>
+    <t>APLLTD</t>
+  </si>
+  <si>
+    <t>PFIZER</t>
+  </si>
+  <si>
+    <t>JBCHEPHARM</t>
+  </si>
+  <si>
+    <t>BIOCON</t>
+  </si>
+  <si>
+    <t>AJANTPHARM</t>
+  </si>
+  <si>
+    <t>IPCALAB</t>
+  </si>
+  <si>
+    <t>GLAXO</t>
+  </si>
+  <si>
+    <t>ABBOTINDIA</t>
+  </si>
+  <si>
+    <t>ALKEM</t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="B358" sqref="B358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1498,7 +1777,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11" t="s">
         <v>137</v>
@@ -1509,18 +1788,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
         <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1536,7 +1815,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B15" t="s">
         <v>138</v>
@@ -1547,13 +1826,13 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B16" t="s">
         <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1569,7 +1848,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1607,13 +1886,13 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B22" t="s">
         <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1629,516 +1908,510 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" t="s">
-        <v>150</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>320</v>
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>269</v>
-      </c>
-      <c r="B26" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" t="s">
-        <v>145</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>267</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>297</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>321</v>
+        <v>295</v>
+      </c>
+      <c r="B29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>268</v>
-      </c>
-      <c r="B30" t="s">
-        <v>151</v>
-      </c>
-      <c r="C30" t="s">
-        <v>152</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>266</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C31" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
         <v>148</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>235</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>322</v>
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" t="s">
-        <v>156</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>272</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
-        <v>304</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>270</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>157</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>267</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s">
         <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
         <v>137</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="B44" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B47" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
       <c r="B48" t="s">
         <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>305</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s">
         <v>148</v>
       </c>
       <c r="C49" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>296</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>164</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>323</v>
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C55" t="s">
-        <v>169</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="B56" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>311</v>
+        <v>66</v>
+      </c>
+      <c r="B58" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>128</v>
-      </c>
-      <c r="B59" t="s">
-        <v>146</v>
-      </c>
-      <c r="C59" t="s">
-        <v>169</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="B62" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>264</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B64" t="s">
         <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>307</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>261</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C65" t="s">
-        <v>175</v>
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="B66" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>178</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>324</v>
+        <v>178</v>
+      </c>
+      <c r="B70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>242</v>
-      </c>
-      <c r="B71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" t="s">
-        <v>171</v>
+        <v>322</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="B72" t="s">
         <v>137</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>262</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C73" t="s">
-        <v>302</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -2154,7 +2427,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
         <v>165</v>
@@ -2198,7 +2471,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B79" t="s">
         <v>148</v>
@@ -2209,7 +2482,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B80" t="s">
         <v>148</v>
@@ -2220,7 +2493,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -2247,29 +2520,29 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B84" t="s">
         <v>138</v>
       </c>
       <c r="C84" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B85" t="s">
         <v>148</v>
       </c>
       <c r="C85" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B86" t="s">
         <v>138</v>
@@ -2291,17 +2564,17 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B90" t="s">
         <v>139</v>
@@ -2312,17 +2585,17 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -2360,17 +2633,17 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -2397,17 +2670,17 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -2434,7 +2707,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -2472,12 +2745,12 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -2515,7 +2788,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -2619,613 +2892,613 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>254</v>
+        <v>19</v>
+      </c>
+      <c r="B127" t="s">
+        <v>151</v>
+      </c>
+      <c r="C127" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>19</v>
-      </c>
-      <c r="B128" t="s">
-        <v>151</v>
-      </c>
-      <c r="C128" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>253</v>
+        <v>133</v>
+      </c>
+      <c r="B129" t="s">
+        <v>138</v>
+      </c>
+      <c r="C129" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>133</v>
-      </c>
-      <c r="B130" t="s">
-        <v>138</v>
-      </c>
-      <c r="C130" t="s">
-        <v>198</v>
+        <v>314</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>316</v>
+        <v>75</v>
+      </c>
+      <c r="B131" t="s">
+        <v>138</v>
+      </c>
+      <c r="C131" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="C132" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B133" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C133" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="B134" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="C134" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>1</v>
-      </c>
-      <c r="B135" t="s">
-        <v>167</v>
-      </c>
-      <c r="C135" t="s">
-        <v>185</v>
+        <v>311</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>313</v>
+        <v>59</v>
+      </c>
+      <c r="B136" t="s">
+        <v>148</v>
+      </c>
+      <c r="C136" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>59</v>
-      </c>
-      <c r="B137" t="s">
-        <v>148</v>
-      </c>
-      <c r="C137" t="s">
-        <v>164</v>
+        <v>288</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>329</v>
+        <v>220</v>
+      </c>
+      <c r="B140" t="s">
+        <v>137</v>
+      </c>
+      <c r="C140" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>220</v>
+        <v>33</v>
       </c>
       <c r="B141" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C141" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B142" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C142" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>34</v>
-      </c>
-      <c r="B143" t="s">
-        <v>138</v>
-      </c>
-      <c r="C143" t="s">
-        <v>187</v>
+        <v>328</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>331</v>
+        <v>287</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>289</v>
+        <v>330</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>332</v>
+        <v>286</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>250</v>
+        <v>285</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>287</v>
+        <v>84</v>
+      </c>
+      <c r="B150" t="s">
+        <v>153</v>
+      </c>
+      <c r="C150" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B151" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C151" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>39</v>
-      </c>
-      <c r="B152" t="s">
-        <v>151</v>
-      </c>
-      <c r="C152" t="s">
-        <v>173</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>317</v>
+        <v>246</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>247</v>
+        <v>312</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>314</v>
+        <v>284</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>286</v>
+        <v>228</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>229</v>
+        <v>22</v>
+      </c>
+      <c r="B158" t="s">
+        <v>151</v>
+      </c>
+      <c r="C158" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>22</v>
-      </c>
-      <c r="B159" t="s">
-        <v>151</v>
-      </c>
-      <c r="C159" t="s">
-        <v>201</v>
+        <v>331</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>333</v>
+        <v>49</v>
+      </c>
+      <c r="B160" t="s">
+        <v>148</v>
+      </c>
+      <c r="C160" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>49</v>
-      </c>
-      <c r="B161" t="s">
-        <v>148</v>
-      </c>
-      <c r="C161" t="s">
-        <v>202</v>
+        <v>332</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>334</v>
+        <v>283</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>251</v>
+        <v>7</v>
+      </c>
+      <c r="B164" t="s">
+        <v>167</v>
+      </c>
+      <c r="C164" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B165" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C165" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="B166" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C166" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>116</v>
       </c>
-      <c r="B167" t="s">
-        <v>138</v>
-      </c>
-      <c r="C167" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>116</v>
+        <v>86</v>
+      </c>
+      <c r="B168" t="s">
+        <v>153</v>
+      </c>
+      <c r="C168" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B169" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C169" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>30</v>
-      </c>
-      <c r="B170" t="s">
-        <v>137</v>
-      </c>
-      <c r="C170" t="s">
-        <v>204</v>
+        <v>281</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>223</v>
+        <v>58</v>
+      </c>
+      <c r="B171" t="s">
+        <v>148</v>
+      </c>
+      <c r="C171" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>283</v>
+        <v>85</v>
+      </c>
+      <c r="B172" t="s">
+        <v>153</v>
+      </c>
+      <c r="C172" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>58</v>
-      </c>
-      <c r="B173" t="s">
-        <v>148</v>
-      </c>
-      <c r="C173" t="s">
-        <v>164</v>
+        <v>280</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B174" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C174" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="B176" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C176" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>281</v>
+        <v>109</v>
+      </c>
+      <c r="B177" t="s">
+        <v>138</v>
+      </c>
+      <c r="C177" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B178" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C178" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>109</v>
-      </c>
-      <c r="B179" t="s">
-        <v>138</v>
-      </c>
-      <c r="C179" t="s">
-        <v>199</v>
+        <v>278</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>111</v>
-      </c>
-      <c r="B180" t="s">
-        <v>138</v>
-      </c>
-      <c r="C180" t="s">
-        <v>199</v>
+        <v>333</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>280</v>
+        <v>6</v>
+      </c>
+      <c r="B181" t="s">
+        <v>167</v>
+      </c>
+      <c r="C181" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>335</v>
+        <v>277</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="B183" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="C183" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>279</v>
+        <v>94</v>
+      </c>
+      <c r="B184" t="s">
+        <v>139</v>
+      </c>
+      <c r="C184" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B185" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C185" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>94</v>
-      </c>
-      <c r="B186" t="s">
-        <v>139</v>
-      </c>
-      <c r="C186" t="s">
-        <v>143</v>
+        <v>290</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B187" t="s">
         <v>138</v>
       </c>
       <c r="C187" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>292</v>
+        <v>25</v>
+      </c>
+      <c r="B188" t="s">
+        <v>151</v>
+      </c>
+      <c r="C188" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>29</v>
-      </c>
-      <c r="B189" t="s">
-        <v>138</v>
-      </c>
-      <c r="C189" t="s">
-        <v>157</v>
+        <v>240</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>25</v>
-      </c>
-      <c r="B190" t="s">
-        <v>151</v>
-      </c>
-      <c r="C190" t="s">
-        <v>201</v>
+        <v>334</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>241</v>
+        <v>103</v>
+      </c>
+      <c r="B191" t="s">
+        <v>137</v>
+      </c>
+      <c r="C191" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>336</v>
+        <v>105</v>
+      </c>
+      <c r="B192" t="s">
+        <v>137</v>
+      </c>
+      <c r="C192" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B193" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C193" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>105</v>
-      </c>
-      <c r="B194" t="s">
-        <v>137</v>
-      </c>
-      <c r="C194" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>102</v>
-      </c>
-      <c r="B195" t="s">
-        <v>138</v>
-      </c>
-      <c r="C195" t="s">
-        <v>199</v>
+        <v>276</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>238</v>
+        <v>96</v>
+      </c>
+      <c r="B196" t="s">
+        <v>139</v>
+      </c>
+      <c r="C196" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="B198" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="C198" t="s">
-        <v>207</v>
+        <v>165</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>277</v>
+        <v>338</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>46</v>
-      </c>
-      <c r="B200" t="s">
-        <v>165</v>
-      </c>
-      <c r="C200" t="s">
-        <v>165</v>
+        <v>274</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>275</v>
+        <v>339</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -3263,7 +3536,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
@@ -3273,7 +3546,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -3311,7 +3584,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -3349,7 +3622,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -3359,7 +3632,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
@@ -3419,7 +3692,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
@@ -3490,179 +3763,713 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>337</v>
+        <v>306</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>308</v>
+        <v>23</v>
+      </c>
+      <c r="B235" t="s">
+        <v>148</v>
+      </c>
+      <c r="C235" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="B236" t="s">
         <v>148</v>
       </c>
       <c r="C236" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>181</v>
+        <v>51</v>
       </c>
       <c r="B237" t="s">
         <v>148</v>
       </c>
       <c r="C237" t="s">
-        <v>217</v>
+        <v>154</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="B238" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C238" t="s">
-        <v>154</v>
+        <v>210</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>126</v>
-      </c>
-      <c r="B239" t="s">
-        <v>137</v>
-      </c>
-      <c r="C239" t="s">
-        <v>188</v>
+        <v>282</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B240" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="C240" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>284</v>
+        <v>69</v>
+      </c>
+      <c r="B241" t="s">
+        <v>137</v>
+      </c>
+      <c r="C241" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B242" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C242" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>69</v>
-      </c>
-      <c r="B243" t="s">
-        <v>137</v>
-      </c>
-      <c r="C243" t="s">
-        <v>204</v>
+        <v>293</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>338</v>
+        <v>132</v>
+      </c>
+      <c r="B244" t="s">
+        <v>139</v>
+      </c>
+      <c r="C244" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>42</v>
-      </c>
-      <c r="B245" t="s">
-        <v>148</v>
-      </c>
-      <c r="C245" t="s">
-        <v>175</v>
+        <v>298</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>132</v>
-      </c>
-      <c r="B247" t="s">
-        <v>139</v>
-      </c>
-      <c r="C247" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>300</v>
+        <v>18</v>
+      </c>
+      <c r="B248" t="s">
+        <v>151</v>
+      </c>
+      <c r="C248" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>294</v>
+        <v>233</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>243</v>
+        <v>127</v>
+      </c>
+      <c r="B250" t="s">
+        <v>146</v>
+      </c>
+      <c r="C250" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>18</v>
-      </c>
-      <c r="B251" t="s">
-        <v>151</v>
-      </c>
-      <c r="C251" t="s">
-        <v>173</v>
+        <v>335</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>234</v>
+        <v>336</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>127</v>
-      </c>
-      <c r="B253" t="s">
-        <v>146</v>
-      </c>
-      <c r="C253" t="s">
-        <v>169</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H153" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C253">
-      <sortCondition ref="A1:A153"/>
+  <autoFilter ref="A1:H152" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C252">
+      <sortCondition ref="A1:A152"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>